<commit_message>
get the proper weights for wcl: 1400,1400, 6250
</commit_message>
<xml_diff>
--- a/notebooks/scripts/all_negative_edges.xlsx
+++ b/notebooks/scripts/all_negative_edges.xlsx
@@ -6927,7 +6927,7 @@
         <v>6250</v>
       </c>
       <c r="Q97" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="98">
@@ -6972,7 +6972,7 @@
         <v>6250</v>
       </c>
       <c r="Q98" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="99">
@@ -7017,7 +7017,7 @@
         <v>6250</v>
       </c>
       <c r="Q99" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="100">
@@ -7062,7 +7062,7 @@
         <v>6250</v>
       </c>
       <c r="Q100" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="101">
@@ -7107,7 +7107,7 @@
         <v>6250</v>
       </c>
       <c r="Q101" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="102">
@@ -7152,7 +7152,7 @@
         <v>6250</v>
       </c>
       <c r="Q102" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="103">
@@ -7197,7 +7197,7 @@
         <v>6250</v>
       </c>
       <c r="Q103" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="104">
@@ -7242,7 +7242,7 @@
         <v>6250</v>
       </c>
       <c r="Q104" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="105">
@@ -7287,7 +7287,7 @@
         <v>6250</v>
       </c>
       <c r="Q105" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="106">
@@ -7332,7 +7332,7 @@
         <v>6250</v>
       </c>
       <c r="Q106" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="107">
@@ -7377,7 +7377,7 @@
         <v>6250</v>
       </c>
       <c r="Q107" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="108">
@@ -7422,7 +7422,7 @@
         <v>6250</v>
       </c>
       <c r="Q108" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="109">
@@ -7467,7 +7467,7 @@
         <v>6250</v>
       </c>
       <c r="Q109" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="110">
@@ -7512,7 +7512,7 @@
         <v>6250</v>
       </c>
       <c r="Q110" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="111">
@@ -7557,7 +7557,7 @@
         <v>6250</v>
       </c>
       <c r="Q111" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="112">
@@ -7602,7 +7602,7 @@
         <v>6250</v>
       </c>
       <c r="Q112" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="113">
@@ -7647,7 +7647,7 @@
         <v>6250</v>
       </c>
       <c r="Q113" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="114">
@@ -7692,7 +7692,7 @@
         <v>6250</v>
       </c>
       <c r="Q114" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="115">
@@ -7737,7 +7737,7 @@
         <v>6250</v>
       </c>
       <c r="Q115" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="116">
@@ -7782,7 +7782,7 @@
         <v>6250</v>
       </c>
       <c r="Q116" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="117">
@@ -7961,7 +7961,7 @@
         <v>6250</v>
       </c>
       <c r="Q119" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="120">
@@ -8006,7 +8006,7 @@
         <v>6250</v>
       </c>
       <c r="Q120" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="121">
@@ -8051,7 +8051,7 @@
         <v>6250</v>
       </c>
       <c r="Q121" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="122">
@@ -8096,7 +8096,7 @@
         <v>6250</v>
       </c>
       <c r="Q122" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="123">
@@ -8141,7 +8141,7 @@
         <v>6250</v>
       </c>
       <c r="Q123" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="124">
@@ -8186,7 +8186,7 @@
         <v>6250</v>
       </c>
       <c r="Q124" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="125">
@@ -8231,7 +8231,7 @@
         <v>6250</v>
       </c>
       <c r="Q125" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="126">
@@ -8276,7 +8276,7 @@
         <v>6250</v>
       </c>
       <c r="Q126" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="127">
@@ -8321,7 +8321,7 @@
         <v>6250</v>
       </c>
       <c r="Q127" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="128">
@@ -8366,7 +8366,7 @@
         <v>6250</v>
       </c>
       <c r="Q128" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="129">
@@ -8411,7 +8411,7 @@
         <v>6250</v>
       </c>
       <c r="Q129" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="130">
@@ -8456,7 +8456,7 @@
         <v>6250</v>
       </c>
       <c r="Q130" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="131">
@@ -8501,7 +8501,7 @@
         <v>6250</v>
       </c>
       <c r="Q131" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="132">
@@ -8546,7 +8546,7 @@
         <v>6250</v>
       </c>
       <c r="Q132" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="133">
@@ -8591,7 +8591,7 @@
         <v>6250</v>
       </c>
       <c r="Q133" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="134">
@@ -8636,7 +8636,7 @@
         <v>6250</v>
       </c>
       <c r="Q134" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="135">
@@ -8681,7 +8681,7 @@
         <v>6250</v>
       </c>
       <c r="Q135" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="136">
@@ -8726,7 +8726,7 @@
         <v>6250</v>
       </c>
       <c r="Q136" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="137">
@@ -8771,7 +8771,7 @@
         <v>6250</v>
       </c>
       <c r="Q137" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="138">
@@ -8816,7 +8816,7 @@
         <v>6250</v>
       </c>
       <c r="Q138" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="139">
@@ -8861,7 +8861,7 @@
         <v>6250</v>
       </c>
       <c r="Q139" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="140">
@@ -8906,7 +8906,7 @@
         <v>6250</v>
       </c>
       <c r="Q140" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="141">
@@ -8951,7 +8951,7 @@
         <v>6250</v>
       </c>
       <c r="Q141" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="142">
@@ -8996,7 +8996,7 @@
         <v>6250</v>
       </c>
       <c r="Q142" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="143">
@@ -9041,7 +9041,7 @@
         <v>6250</v>
       </c>
       <c r="Q143" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="144">
@@ -9086,7 +9086,7 @@
         <v>6250</v>
       </c>
       <c r="Q144" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="145">
@@ -9131,7 +9131,7 @@
         <v>6250</v>
       </c>
       <c r="Q145" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="146">
@@ -9176,7 +9176,7 @@
         <v>6250</v>
       </c>
       <c r="Q146" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="147">
@@ -9221,7 +9221,7 @@
         <v>6250</v>
       </c>
       <c r="Q147" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="148">
@@ -9266,7 +9266,7 @@
         <v>6250</v>
       </c>
       <c r="Q148" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="149">
@@ -9311,7 +9311,7 @@
         <v>6250</v>
       </c>
       <c r="Q149" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="150">
@@ -9356,7 +9356,7 @@
         <v>6250</v>
       </c>
       <c r="Q150" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="151">
@@ -9401,7 +9401,7 @@
         <v>6250</v>
       </c>
       <c r="Q151" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="152">
@@ -9446,7 +9446,7 @@
         <v>6250</v>
       </c>
       <c r="Q152" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="153">
@@ -9491,7 +9491,7 @@
         <v>6250</v>
       </c>
       <c r="Q153" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="154">
@@ -9536,7 +9536,7 @@
         <v>6250</v>
       </c>
       <c r="Q154" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="155">
@@ -9581,7 +9581,7 @@
         <v>6250</v>
       </c>
       <c r="Q155" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="156">
@@ -9626,7 +9626,7 @@
         <v>6250</v>
       </c>
       <c r="Q156" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="157">
@@ -9671,7 +9671,7 @@
         <v>6250</v>
       </c>
       <c r="Q157" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="158">
@@ -9716,7 +9716,7 @@
         <v>6250</v>
       </c>
       <c r="Q158" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="159">
@@ -9761,7 +9761,7 @@
         <v>6250</v>
       </c>
       <c r="Q159" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="160">
@@ -9806,7 +9806,7 @@
         <v>6250</v>
       </c>
       <c r="Q160" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="161">
@@ -9851,7 +9851,7 @@
         <v>6250</v>
       </c>
       <c r="Q161" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="162">
@@ -9896,7 +9896,7 @@
         <v>6250</v>
       </c>
       <c r="Q162" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="163">
@@ -9941,7 +9941,7 @@
         <v>6250</v>
       </c>
       <c r="Q163" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="164">
@@ -9986,7 +9986,7 @@
         <v>6250</v>
       </c>
       <c r="Q164" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="165">
@@ -10031,7 +10031,7 @@
         <v>6250</v>
       </c>
       <c r="Q165" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="166">
@@ -10076,7 +10076,7 @@
         <v>6250</v>
       </c>
       <c r="Q166" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="167">
@@ -10121,7 +10121,7 @@
         <v>6250</v>
       </c>
       <c r="Q167" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="168">
@@ -10166,7 +10166,7 @@
         <v>6250</v>
       </c>
       <c r="Q168" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="169">
@@ -10211,7 +10211,7 @@
         <v>6250</v>
       </c>
       <c r="Q169" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="170">
@@ -10256,7 +10256,7 @@
         <v>6250</v>
       </c>
       <c r="Q170" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="171">
@@ -10301,7 +10301,7 @@
         <v>6250</v>
       </c>
       <c r="Q171" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>